<commit_message>
level correction applied to all apadec stations
</commit_message>
<xml_diff>
--- a/data-raw/Level to Depth conversions.xlsx
+++ b/data-raw/Level to Depth conversions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Palandri_M\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\nerrs-metabolism\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6F8EEB-8D3A-4A57-874F-82566870E77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0F687E-6595-40EB-B1A2-6A712D4724E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3ADF06CF-836C-499A-8CD5-6122F616C132}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3ADF06CF-836C-499A-8CD5-6122F616C132}"/>
   </bookViews>
   <sheets>
     <sheet name="Cat Point" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
   <si>
     <t>Site: Cat Point</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>Site: East Bay Bottom</t>
-  </si>
-  <si>
-    <t>2:15 (last reading)</t>
   </si>
   <si>
     <t>Subtract from Level Values</t>
@@ -117,28 +114,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -476,7 +465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3113006F-689F-4FA3-B563-04F039750796}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A31" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -510,7 +499,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -527,7 +516,7 @@
         <v>0.40625</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -543,7 +532,7 @@
       <c r="D4" s="2">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -560,7 +549,7 @@
       <c r="D5" s="2">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -577,7 +566,7 @@
       <c r="D6" s="2">
         <v>0.44791666666666669</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -594,7 +583,7 @@
       <c r="D7" s="2">
         <v>0.63541666666666663</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -611,7 +600,7 @@
       <c r="D8" s="2">
         <v>0.34375</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -628,7 +617,7 @@
       <c r="D9" s="2">
         <v>0.76041666666666663</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -645,7 +634,7 @@
       <c r="D10" s="2">
         <v>0.35416666666666669</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -662,7 +651,7 @@
       <c r="D11" s="2">
         <v>0.36458333333333331</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -679,7 +668,7 @@
       <c r="D12" s="2">
         <v>0.33333333333333331</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -696,7 +685,7 @@
       <c r="D13" s="2">
         <v>0.34375</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -713,7 +702,7 @@
       <c r="D14" s="2">
         <v>0.51041666666666663</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -730,7 +719,7 @@
       <c r="D15" s="2">
         <v>0.4375</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -747,7 +736,7 @@
       <c r="D16" s="2">
         <v>0.51041666666666663</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -764,7 +753,7 @@
       <c r="D17" s="2">
         <v>0.51041666666666663</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -781,7 +770,7 @@
       <c r="D18" s="2">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -798,7 +787,7 @@
       <c r="D19" s="2">
         <v>0.4375</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -815,7 +804,7 @@
       <c r="D20" s="2">
         <v>0.36458333333333331</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -832,7 +821,7 @@
       <c r="D21" s="2">
         <v>0.46875</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -849,7 +838,7 @@
       <c r="D22" s="2">
         <v>0.36458333333333331</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -866,7 +855,7 @@
       <c r="D23" s="2">
         <v>0.375</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -883,7 +872,7 @@
       <c r="D24" s="2">
         <v>0.33333333333333331</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -900,7 +889,7 @@
       <c r="D25" s="2">
         <v>0.38541666666666669</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -917,7 +906,7 @@
       <c r="D26" s="2">
         <v>0.4375</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -934,7 +923,7 @@
       <c r="D27" s="2">
         <v>0.375</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -951,7 +940,7 @@
       <c r="D28" s="2">
         <v>0.44791666666666669</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -968,7 +957,7 @@
       <c r="D29" s="2">
         <v>0.38541666666666669</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -985,7 +974,7 @@
       <c r="D30" s="2">
         <v>0.38541666666666669</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -1002,7 +991,7 @@
       <c r="D31" s="2">
         <v>0.42708333333333331</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -1019,7 +1008,7 @@
       <c r="D32" s="2">
         <v>0.5625</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -1036,7 +1025,7 @@
       <c r="D33" s="2">
         <v>0.59375</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -1053,7 +1042,7 @@
       <c r="D34" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -1070,7 +1059,7 @@
       <c r="D35" s="4">
         <v>0.46875</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35">
         <v>-1.6830000000000001</v>
       </c>
     </row>
@@ -1104,7 +1093,7 @@
       <c r="D37" s="4">
         <v>0.39583333333333331</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37">
         <v>-1.782</v>
       </c>
     </row>
@@ -1121,7 +1110,7 @@
       <c r="D38" s="4">
         <v>0.38541666666666669</v>
       </c>
-      <c r="E38" s="7">
+      <c r="E38">
         <v>-1.782</v>
       </c>
     </row>
@@ -1138,7 +1127,7 @@
       <c r="D39" s="4">
         <v>0.44791666666666669</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39">
         <v>-1.782</v>
       </c>
     </row>
@@ -1155,7 +1144,7 @@
       <c r="D40" s="4">
         <v>0.3125</v>
       </c>
-      <c r="E40" s="7">
+      <c r="E40">
         <v>-1.782</v>
       </c>
     </row>
@@ -1172,7 +1161,7 @@
       <c r="D41" s="4">
         <v>0.35416666666666669</v>
       </c>
-      <c r="E41" s="7">
+      <c r="E41">
         <v>-1.782</v>
       </c>
     </row>
@@ -1189,7 +1178,7 @@
       <c r="D42" s="4">
         <v>0.35416666666666669</v>
       </c>
-      <c r="E42" s="7">
+      <c r="E42">
         <v>-1.782</v>
       </c>
     </row>
@@ -1206,7 +1195,7 @@
       <c r="D43" s="4">
         <v>0.375</v>
       </c>
-      <c r="E43" s="7">
+      <c r="E43">
         <v>-1.782</v>
       </c>
     </row>
@@ -1223,7 +1212,7 @@
       <c r="D44" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E44" s="7">
+      <c r="E44">
         <v>-1.782</v>
       </c>
     </row>
@@ -1240,7 +1229,7 @@
       <c r="D45" s="4">
         <v>0.40625</v>
       </c>
-      <c r="E45" s="7">
+      <c r="E45">
         <v>-1.782</v>
       </c>
     </row>
@@ -1257,7 +1246,7 @@
       <c r="D46" s="4">
         <v>0.39583333333333331</v>
       </c>
-      <c r="E46" s="7">
+      <c r="E46">
         <v>-1.782</v>
       </c>
     </row>
@@ -1274,7 +1263,7 @@
       <c r="D47" s="4">
         <v>0.44791666666666669</v>
       </c>
-      <c r="E47" s="7">
+      <c r="E47">
         <v>-1.782</v>
       </c>
     </row>
@@ -1291,7 +1280,7 @@
       <c r="D48" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="E48" s="7">
+      <c r="E48">
         <v>-1.782</v>
       </c>
     </row>
@@ -1304,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E61F5AA-80C1-4B56-9728-12BAEDADDFBA}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1340,8 +1329,8 @@
       <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>8</v>
+      <c r="E2" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="F2" s="5"/>
     </row>
@@ -1359,7 +1348,7 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1375,7 +1364,7 @@
       <c r="D4" s="4">
         <v>0.47916666666666669</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1392,7 +1381,7 @@
       <c r="D5" s="4">
         <v>0.53125</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1409,7 +1398,7 @@
       <c r="D6" s="4">
         <v>0.36458333333333331</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1426,7 +1415,7 @@
       <c r="D7" s="4">
         <v>0.60416666666666663</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1443,7 +1432,7 @@
       <c r="D8" s="4">
         <v>0.4375</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1460,7 +1449,7 @@
       <c r="D9" s="4">
         <v>0.4375</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1477,7 +1466,7 @@
       <c r="D10" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1494,7 +1483,7 @@
       <c r="D11" s="4">
         <v>0.3125</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1511,7 +1500,7 @@
       <c r="D12" s="4">
         <v>0.40625</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1528,7 +1517,7 @@
       <c r="D13" s="4">
         <v>0.40625</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1545,7 +1534,7 @@
       <c r="D14" s="4">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1562,7 +1551,7 @@
       <c r="D15" s="4">
         <v>0.36458333333333331</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1579,7 +1568,7 @@
       <c r="D16" s="4">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1596,7 +1585,7 @@
       <c r="D17" s="4">
         <v>0.59375</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1613,7 +1602,7 @@
       <c r="D18" s="4">
         <v>0.52083333333333337</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1630,7 +1619,7 @@
       <c r="D19" s="4">
         <v>0.375</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1647,7 +1636,7 @@
       <c r="D20" s="4">
         <v>0.44791666666666669</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1664,7 +1653,7 @@
       <c r="D21" s="4">
         <v>0.53125</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1681,7 +1670,7 @@
       <c r="D22" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1698,7 +1687,7 @@
       <c r="D23" s="4">
         <v>0.47916666666666669</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1715,7 +1704,7 @@
       <c r="D24" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1732,7 +1721,7 @@
       <c r="D25" s="4">
         <v>0.36458333333333331</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1749,7 +1738,7 @@
       <c r="D26" s="4">
         <v>0.3125</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1766,7 +1755,7 @@
       <c r="D27" s="4">
         <v>0.35416666666666669</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1783,7 +1772,7 @@
       <c r="D28" s="4">
         <v>0.30208333333333331</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E28">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1800,7 +1789,7 @@
       <c r="D29" s="4">
         <v>0.35416666666666669</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E29">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1817,7 +1806,7 @@
       <c r="D30" s="4">
         <v>0.30208333333333331</v>
       </c>
-      <c r="E30" s="8">
+      <c r="E30">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1834,7 +1823,7 @@
       <c r="D31" s="4">
         <v>0.44791666666666669</v>
       </c>
-      <c r="E31" s="8">
+      <c r="E31">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1851,7 +1840,7 @@
       <c r="D32" s="4">
         <v>0.48958333333333331</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E32">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1868,7 +1857,7 @@
       <c r="D33" s="4">
         <v>0.61458333333333337</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E33">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1885,7 +1874,7 @@
       <c r="D34" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E34" s="8">
+      <c r="E34">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1902,7 +1891,7 @@
       <c r="D35" s="4">
         <v>0.44791666666666669</v>
       </c>
-      <c r="E35" s="8">
+      <c r="E35">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1919,7 +1908,7 @@
       <c r="D36" s="4">
         <v>0.48958333333333331</v>
       </c>
-      <c r="E36" s="8">
+      <c r="E36">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1936,7 +1925,7 @@
       <c r="D37" s="4">
         <v>0.375</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E37">
         <v>-1.3919999999999999</v>
       </c>
     </row>
@@ -1967,10 +1956,10 @@
       <c r="C39" s="3">
         <v>45393</v>
       </c>
-      <c r="D39" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="8">
+      <c r="D39" s="4">
+        <v>9.375E-2</v>
+      </c>
+      <c r="E39">
         <v>-1.4610000000000001</v>
       </c>
     </row>
@@ -1987,7 +1976,7 @@
       <c r="D40" s="4">
         <v>0.30208333333333331</v>
       </c>
-      <c r="E40" s="8">
+      <c r="E40">
         <v>-1.4610000000000001</v>
       </c>
     </row>
@@ -2004,7 +1993,7 @@
       <c r="D41" s="4">
         <v>0.34375</v>
       </c>
-      <c r="E41" s="8">
+      <c r="E41">
         <v>-1.4610000000000001</v>
       </c>
     </row>
@@ -2021,7 +2010,7 @@
       <c r="D42" s="4">
         <v>0.36458333333333331</v>
       </c>
-      <c r="E42" s="8">
+      <c r="E42">
         <v>-1.4610000000000001</v>
       </c>
     </row>
@@ -2038,7 +2027,7 @@
       <c r="D43" s="4">
         <v>0.30208333333333331</v>
       </c>
-      <c r="E43" s="8">
+      <c r="E43">
         <v>-1.4610000000000001</v>
       </c>
     </row>
@@ -2055,7 +2044,7 @@
       <c r="D44" s="4">
         <v>0.30208333333333331</v>
       </c>
-      <c r="E44" s="8">
+      <c r="E44">
         <v>-1.4610000000000001</v>
       </c>
     </row>
@@ -2072,7 +2061,7 @@
       <c r="D45" s="4">
         <v>0.32291666666666669</v>
       </c>
-      <c r="E45" s="8">
+      <c r="E45">
         <v>-1.4610000000000001</v>
       </c>
     </row>
@@ -2089,7 +2078,7 @@
       <c r="D46" s="4">
         <v>0.48958333333333331</v>
       </c>
-      <c r="E46" s="8">
+      <c r="E46">
         <v>-1.4610000000000001</v>
       </c>
     </row>
@@ -2106,7 +2095,7 @@
       <c r="D47" s="4">
         <v>0.48958333333333331</v>
       </c>
-      <c r="E47" s="8">
+      <c r="E47">
         <v>-1.4610000000000001</v>
       </c>
     </row>
@@ -2123,7 +2112,7 @@
       <c r="D48" s="4">
         <v>0.34375</v>
       </c>
-      <c r="E48" s="8">
+      <c r="E48">
         <v>-1.4610000000000001</v>
       </c>
     </row>
@@ -2140,7 +2129,7 @@
       <c r="D49" s="4">
         <v>0.5625</v>
       </c>
-      <c r="E49" s="8">
+      <c r="E49">
         <v>-1.4610000000000001</v>
       </c>
     </row>
@@ -2188,8 +2177,8 @@
       <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>8</v>
+      <c r="E2" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2206,7 +2195,7 @@
         <v>0.36458333333333331</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2222,7 +2211,7 @@
       <c r="D4" s="4">
         <v>0.375</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2239,7 +2228,7 @@
       <c r="D5" s="4">
         <v>0.36458333333333331</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2256,7 +2245,7 @@
       <c r="D6" s="4">
         <v>0.48958333333333331</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2273,7 +2262,7 @@
       <c r="D7" s="4">
         <v>0.60416666666666663</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2290,7 +2279,7 @@
       <c r="D8" s="4">
         <v>0.3125</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2307,7 +2296,7 @@
       <c r="D9" s="4">
         <v>0.32291666666666669</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2324,7 +2313,7 @@
       <c r="D10" s="4">
         <v>0.38541666666666669</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2341,7 +2330,7 @@
       <c r="D11" s="4">
         <v>0.39583333333333331</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2358,7 +2347,7 @@
       <c r="D12" s="4">
         <v>0.30208333333333331</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2375,7 +2364,7 @@
       <c r="D13" s="4">
         <v>0.3125</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2392,7 +2381,7 @@
       <c r="D14" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2409,7 +2398,7 @@
       <c r="D15" s="4">
         <v>0.35416666666666669</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2426,7 +2415,7 @@
       <c r="D16" s="4">
         <v>0.47916666666666669</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2443,7 +2432,7 @@
       <c r="D17" s="4">
         <v>0.45833333333333331</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2460,7 +2449,7 @@
       <c r="D18" s="4">
         <v>0.375</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2477,7 +2466,7 @@
       <c r="D19" s="4">
         <v>0.35416666666666669</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2494,7 +2483,7 @@
       <c r="D20" s="4">
         <v>0.33333333333333331</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2511,7 +2500,7 @@
       <c r="D21" s="4">
         <v>0.4375</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2528,7 +2517,7 @@
       <c r="D22" s="4">
         <v>0.32291666666666669</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2545,7 +2534,7 @@
       <c r="D23" s="4">
         <v>0.32291666666666669</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2562,7 +2551,7 @@
       <c r="D24" s="4">
         <v>0.29166666666666669</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2579,7 +2568,7 @@
       <c r="D25" s="4">
         <v>0.4375</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2596,7 +2585,7 @@
       <c r="D26" s="4">
         <v>0.45833333333333331</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E26">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2613,7 +2602,7 @@
       <c r="D27" s="4">
         <v>0.39583333333333331</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2630,7 +2619,7 @@
       <c r="D28" s="4">
         <v>0.48958333333333331</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E28">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2647,7 +2636,7 @@
       <c r="D29" s="4">
         <v>0.38541666666666669</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2664,7 +2653,7 @@
       <c r="D30" s="4">
         <v>0.33333333333333331</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E30">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2681,7 +2670,7 @@
       <c r="D31" s="4">
         <v>0.39583333333333331</v>
       </c>
-      <c r="E31" s="10">
+      <c r="E31">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2698,7 +2687,7 @@
       <c r="D32" s="4">
         <v>0.36458333333333331</v>
       </c>
-      <c r="E32" s="10">
+      <c r="E32">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2715,7 +2704,7 @@
       <c r="D33" s="4">
         <v>0.35416666666666669</v>
       </c>
-      <c r="E33" s="10">
+      <c r="E33">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2732,7 +2721,7 @@
       <c r="D34" s="4">
         <v>0.39583333333333331</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E34">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2749,7 +2738,7 @@
       <c r="D35" s="4">
         <v>0.51041666666666663</v>
       </c>
-      <c r="E35" s="10">
+      <c r="E35">
         <v>-1.6919999999999999</v>
       </c>
     </row>
@@ -2783,7 +2772,7 @@
       <c r="D37" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E37" s="10">
+      <c r="E37">
         <v>-1.609</v>
       </c>
     </row>
@@ -2800,7 +2789,7 @@
       <c r="D38" s="4">
         <v>0.40625</v>
       </c>
-      <c r="E38" s="10">
+      <c r="E38">
         <v>-1.609</v>
       </c>
     </row>
@@ -2817,7 +2806,7 @@
       <c r="D39" s="4">
         <v>0.46875</v>
       </c>
-      <c r="E39" s="10">
+      <c r="E39">
         <v>-1.609</v>
       </c>
     </row>
@@ -2834,7 +2823,7 @@
       <c r="D40" s="4">
         <v>0.28125</v>
       </c>
-      <c r="E40" s="10">
+      <c r="E40">
         <v>-1.609</v>
       </c>
     </row>
@@ -2851,7 +2840,7 @@
       <c r="D41" s="4">
         <v>0.38541666666666669</v>
       </c>
-      <c r="E41" s="10">
+      <c r="E41">
         <v>-1.609</v>
       </c>
     </row>
@@ -2868,7 +2857,7 @@
       <c r="D42" s="4">
         <v>0.375</v>
       </c>
-      <c r="E42" s="10">
+      <c r="E42">
         <v>-1.609</v>
       </c>
     </row>
@@ -2885,7 +2874,7 @@
       <c r="D43" s="4">
         <v>0.4375</v>
       </c>
-      <c r="E43" s="10">
+      <c r="E43">
         <v>-1.609</v>
       </c>
     </row>
@@ -2902,7 +2891,7 @@
       <c r="D44" s="4">
         <v>0.375</v>
       </c>
-      <c r="E44" s="10">
+      <c r="E44">
         <v>-1.609</v>
       </c>
     </row>
@@ -2919,7 +2908,7 @@
       <c r="D45" s="4">
         <v>0.36458333333333331</v>
       </c>
-      <c r="E45" s="10">
+      <c r="E45">
         <v>-1.609</v>
       </c>
     </row>
@@ -2936,7 +2925,7 @@
       <c r="D46" s="4">
         <v>0.47916666666666669</v>
       </c>
-      <c r="E46" s="10">
+      <c r="E46">
         <v>-1.609</v>
       </c>
     </row>
@@ -2953,7 +2942,7 @@
       <c r="D47" s="4">
         <v>0.375</v>
       </c>
-      <c r="E47" s="10">
+      <c r="E47">
         <v>-1.609</v>
       </c>
     </row>

</xml_diff>